<commit_message>
predator - whole game can be skipped apparently
</commit_message>
<xml_diff>
--- a/Predator/FrameCompare.xlsx
+++ b/Predator/FrameCompare.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\Predator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF078257-ABA0-4905-BA00-524DE60F34C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0626B20-1305-4484-B78D-6D7BCC331347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42270" yWindow="1005" windowWidth="12015" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V1" sheetId="7" r:id="rId1"/>
+    <sheet name="V2" sheetId="8" r:id="rId1"/>
+    <sheet name="V1" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>Place</t>
   </si>
@@ -72,6 +73,93 @@
   </si>
   <si>
     <t>Big Mode 1 ends (black)</t>
+  </si>
+  <si>
+    <t>Hit 1</t>
+  </si>
+  <si>
+    <t>Hit 2</t>
+  </si>
+  <si>
+    <t>Hit 3</t>
+  </si>
+  <si>
+    <t>Hit 4</t>
+  </si>
+  <si>
+    <t>Hit 5</t>
+  </si>
+  <si>
+    <t>Hit 6</t>
+  </si>
+  <si>
+    <t>Hit 7</t>
+  </si>
+  <si>
+    <t>Hit 8</t>
+  </si>
+  <si>
+    <t>Big Mode 2 appears</t>
+  </si>
+  <si>
+    <t>Big Mode 2 ends (black)</t>
+  </si>
+  <si>
+    <t>Boss health appears</t>
+  </si>
+  <si>
+    <t>Big Mode 3 appears</t>
+  </si>
+  <si>
+    <t>Big Mode 3 ends (black)</t>
+  </si>
+  <si>
+    <t>Big Mode 5 appears</t>
+  </si>
+  <si>
+    <t>Progress 0x05</t>
+  </si>
+  <si>
+    <t>Porgress 0x02</t>
+  </si>
+  <si>
+    <t>Porgress 0x03</t>
+  </si>
+  <si>
+    <t>Porgress 0x04</t>
+  </si>
+  <si>
+    <t>Progress 0x0C</t>
+  </si>
+  <si>
+    <t>Porgress 0x06</t>
+  </si>
+  <si>
+    <t>Porgress 0x07</t>
+  </si>
+  <si>
+    <t>Porgress 0x08</t>
+  </si>
+  <si>
+    <t>Porgress 0x09</t>
+  </si>
+  <si>
+    <t>Porgress 0x0A</t>
+  </si>
+  <si>
+    <t>Porgress 0x0B</t>
+  </si>
+  <si>
+    <t>Progress 0x0D</t>
+  </si>
+  <si>
+    <t>Progress 0x0E</t>
+  </si>
+  <si>
+    <t>Progress 0x0F</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -217,12 +305,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -239,7 +336,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,6 +351,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -573,12 +674,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
-  <dimension ref="A1:F220"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F75CE0-A1C1-4DE3-8C32-09CA7DE610E7}">
+  <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -613,7 +714,7 @@
         <v>90</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D79" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <f t="shared" ref="D2:D102" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>1</v>
       </c>
       <c r="F2" s="2"/>
@@ -634,586 +735,512 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>12</v>
+      <c r="A4" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>3632</v>
+        <v>5588</v>
       </c>
       <c r="C4" s="2">
-        <v>4751</v>
+        <v>12879</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>1119</v>
+        <v>7291</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4564</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5653</v>
-      </c>
-      <c r="D5" s="3">
-        <f t="shared" ref="D5" si="1">IF(C5&lt;&gt;"",IF(B5&lt;&gt;"",C5-B5,"-"), "-")</f>
-        <v>1089</v>
-      </c>
+      <c r="A5" s="13"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3" t="str">
+        <f>IF(E19&lt;&gt;"",IF(B19&lt;&gt;"",E19-B19,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3" t="str">
+        <f>IF(E20&lt;&gt;"",IF(B20&lt;&gt;"",E20-B20,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="3" t="str">
+        <f>IF(E21&lt;&gt;"",IF(B21&lt;&gt;"",E21-B21,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3" t="str">
+        <f>IF(E22&lt;&gt;"",IF(B22&lt;&gt;"",E22-B22,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3" t="str">
+        <f t="shared" ref="F23:F33" si="1">IF(E23&lt;&gt;"",IF(B23&lt;&gt;"",E23-B23,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="2"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16"/>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
-        <v>4</v>
-      </c>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
-        <v>6</v>
-      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="3" t="str">
@@ -1343,7 +1370,7 @@
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="3" t="str">
-        <f t="shared" ref="D80:D81" si="2">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",B80-C80,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1352,7 +1379,7 @@
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1360,125 +1387,240 @@
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
+      <c r="D82" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
+      <c r="D83" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
+      <c r="D84" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
+      <c r="D85" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
+      <c r="D86" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
+      <c r="D87" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
+      <c r="D88" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
+      <c r="D89" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
+      <c r="D90" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
+      <c r="D91" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
+      <c r="D92" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
+      <c r="D93" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
+      <c r="D94" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
+      <c r="D95" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
-    </row>
-    <row r="97" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D96" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
-    </row>
-    <row r="98" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D97" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
-    </row>
-    <row r="99" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D98" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
-    </row>
-    <row r="100" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D99" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
-    </row>
-    <row r="101" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D100" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
-    </row>
-    <row r="102" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D101" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
-    </row>
-    <row r="103" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D102" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
-    </row>
-    <row r="104" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D103" s="3" t="str">
+        <f t="shared" ref="D103:D104" si="2">IF(C103&lt;&gt;"",IF(B103&lt;&gt;"",B103-C103,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
-    </row>
-    <row r="105" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
     </row>
@@ -1913,6 +2055,1875 @@
     <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
+    </row>
+    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+    </row>
+    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+    </row>
+    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+    </row>
+    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="5"/>
+      <c r="C224" s="5"/>
+    </row>
+    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="5"/>
+      <c r="C225" s="5"/>
+    </row>
+    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="5"/>
+      <c r="C226" s="5"/>
+    </row>
+    <row r="227" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+    </row>
+    <row r="228" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+    </row>
+    <row r="229" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="5"/>
+      <c r="C229" s="5"/>
+    </row>
+    <row r="230" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="5"/>
+      <c r="C230" s="5"/>
+    </row>
+    <row r="231" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="5"/>
+      <c r="C231" s="5"/>
+    </row>
+    <row r="232" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+    </row>
+    <row r="233" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="5"/>
+      <c r="C233" s="5"/>
+    </row>
+    <row r="234" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="5"/>
+      <c r="C234" s="5"/>
+    </row>
+    <row r="235" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="5"/>
+      <c r="C235" s="5"/>
+    </row>
+    <row r="236" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="5"/>
+      <c r="C236" s="5"/>
+    </row>
+    <row r="237" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="5"/>
+      <c r="C237" s="5"/>
+    </row>
+    <row r="238" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="5"/>
+      <c r="C238" s="5"/>
+    </row>
+    <row r="239" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="5"/>
+      <c r="C239" s="5"/>
+    </row>
+    <row r="240" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="5"/>
+      <c r="C240" s="5"/>
+    </row>
+    <row r="241" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="5"/>
+      <c r="C241" s="5"/>
+    </row>
+    <row r="242" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="5"/>
+      <c r="C242" s="5"/>
+    </row>
+    <row r="243" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="5"/>
+      <c r="C243" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A88CD45-A2B6-49C4-A4B2-BB74C4A0A2BD}">
+  <dimension ref="A1:F243"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.25" customWidth="1"/>
+    <col min="2" max="3" width="8.75" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>89</v>
+      </c>
+      <c r="C2" s="2">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:F102" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1149</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2070</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" si="0"/>
+        <v>921</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3632</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4751</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3634</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4754</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3730</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4850</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3826</v>
+      </c>
+      <c r="C7" s="2">
+        <v>4945</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3923</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5043</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4018</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5139</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4115</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5236</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4210</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5332</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4306</v>
+      </c>
+      <c r="C12" s="2">
+        <v>5427</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15">
+        <v>4532</v>
+      </c>
+      <c r="C13" s="15">
+        <v>5653</v>
+      </c>
+      <c r="D13" s="16">
+        <f t="shared" ref="D13" si="1">IF(C13&lt;&gt;"",IF(B13&lt;&gt;"",C13-B13,"-"), "-")</f>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4936</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6057</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7547</v>
+      </c>
+      <c r="C15" s="2">
+        <v>8711</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7561</v>
+      </c>
+      <c r="C16" s="2">
+        <v>8728</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="2">
+        <v>8234</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9422</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="15">
+        <v>8459</v>
+      </c>
+      <c r="C18" s="15">
+        <v>9648</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="0"/>
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2">
+        <v>9015</v>
+      </c>
+      <c r="C19" s="2">
+        <v>10204</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>1189</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9015</v>
+      </c>
+      <c r="F19" s="3">
+        <f>IF(E19&lt;&gt;"",IF(B19&lt;&gt;"",E19-B19,"-"), "-")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2">
+        <v>9041</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2">
+        <v>9041</v>
+      </c>
+      <c r="F20" s="3">
+        <f>IF(E20&lt;&gt;"",IF(B20&lt;&gt;"",E20-B20,"-"), "-")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2">
+        <v>9157</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2">
+        <v>9171</v>
+      </c>
+      <c r="F21" s="3">
+        <f>IF(E21&lt;&gt;"",IF(B21&lt;&gt;"",E21-B21,"-"), "-")</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2">
+        <v>9454</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2">
+        <v>9455</v>
+      </c>
+      <c r="F22" s="3">
+        <f>IF(E22&lt;&gt;"",IF(B22&lt;&gt;"",E22-B22,"-"), "-")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2">
+        <v>9576</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2">
+        <v>9866</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" ref="F23:F33" si="2">IF(E23&lt;&gt;"",IF(B23&lt;&gt;"",E23-B23,"-"), "-")</f>
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="2">
+        <v>10023</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2">
+        <v>10022</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10025</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="2">
+        <v>10091</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="2">
+        <v>10249</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="2">
+        <v>10319</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="13">
+        <v>10429</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="2">
+        <v>10496</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2">
+        <v>10431</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="2">
+        <v>10730</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2">
+        <v>10833</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="2">
+        <v>10731</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>-102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="2">
+        <v>11095</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="2">
+        <v>11579</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="2">
+        <v>11582</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2">
+        <v>11583</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2">
+        <v>11481</v>
+      </c>
+      <c r="C34" s="2">
+        <v>12425</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>944</v>
+      </c>
+      <c r="E34" s="13">
+        <v>11583</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="2">
+        <v>13362</v>
+      </c>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15">
+        <v>13588</v>
+      </c>
+      <c r="D36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2">
+        <v>13992</v>
+      </c>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="11"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2">
+        <v>12879</v>
+      </c>
+      <c r="C44" s="2">
+        <v>24472</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>11593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="11"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5"/>
+      <c r="B84" s="5"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="5"/>
+      <c r="D92" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="5"/>
+      <c r="D94" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="5"/>
+      <c r="D95" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="5"/>
+      <c r="D97" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="5"/>
+      <c r="D98" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="5"/>
+      <c r="D99" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="5"/>
+      <c r="D100" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="5"/>
+      <c r="D101" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="5"/>
+      <c r="D102" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="5"/>
+      <c r="D103" s="3" t="str">
+        <f t="shared" ref="D103:D104" si="3">IF(C103&lt;&gt;"",IF(B103&lt;&gt;"",B103-C103,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
+      <c r="C106" s="5"/>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5"/>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="C109" s="5"/>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+    </row>
+    <row r="113" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+    </row>
+    <row r="114" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+    </row>
+    <row r="115" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+    </row>
+    <row r="116" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+    </row>
+    <row r="117" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="C117" s="5"/>
+    </row>
+    <row r="118" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5"/>
+    </row>
+    <row r="119" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+    </row>
+    <row r="120" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+    </row>
+    <row r="121" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="5"/>
+    </row>
+    <row r="122" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+    </row>
+    <row r="123" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+    </row>
+    <row r="124" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="5"/>
+    </row>
+    <row r="125" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+    </row>
+    <row r="126" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+    </row>
+    <row r="127" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B127" s="5"/>
+      <c r="C127" s="5"/>
+    </row>
+    <row r="128" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="C128" s="5"/>
+    </row>
+    <row r="129" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B129" s="5"/>
+      <c r="C129" s="5"/>
+    </row>
+    <row r="130" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="C130" s="5"/>
+    </row>
+    <row r="131" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="C131" s="5"/>
+    </row>
+    <row r="132" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+    </row>
+    <row r="133" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+    </row>
+    <row r="134" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B134" s="5"/>
+      <c r="C134" s="5"/>
+    </row>
+    <row r="135" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B135" s="5"/>
+      <c r="C135" s="5"/>
+    </row>
+    <row r="136" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+    </row>
+    <row r="137" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+    </row>
+    <row r="138" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B138" s="5"/>
+      <c r="C138" s="5"/>
+    </row>
+    <row r="139" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B139" s="5"/>
+      <c r="C139" s="5"/>
+    </row>
+    <row r="140" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B140" s="5"/>
+      <c r="C140" s="5"/>
+    </row>
+    <row r="141" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B141" s="5"/>
+      <c r="C141" s="5"/>
+    </row>
+    <row r="142" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="5"/>
+      <c r="C142" s="5"/>
+    </row>
+    <row r="143" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5"/>
+    </row>
+    <row r="144" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B144" s="5"/>
+      <c r="C144" s="5"/>
+    </row>
+    <row r="145" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B145" s="5"/>
+      <c r="C145" s="5"/>
+    </row>
+    <row r="146" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B146" s="5"/>
+      <c r="C146" s="5"/>
+    </row>
+    <row r="147" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B147" s="5"/>
+      <c r="C147" s="5"/>
+    </row>
+    <row r="148" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="C148" s="5"/>
+    </row>
+    <row r="149" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B149" s="5"/>
+      <c r="C149" s="5"/>
+    </row>
+    <row r="150" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="C150" s="5"/>
+    </row>
+    <row r="151" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B151" s="5"/>
+      <c r="C151" s="5"/>
+    </row>
+    <row r="152" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="C152" s="5"/>
+    </row>
+    <row r="153" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
+    </row>
+    <row r="154" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="C154" s="5"/>
+    </row>
+    <row r="155" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B155" s="5"/>
+      <c r="C155" s="5"/>
+    </row>
+    <row r="156" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B156" s="5"/>
+      <c r="C156" s="5"/>
+    </row>
+    <row r="157" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B157" s="5"/>
+      <c r="C157" s="5"/>
+    </row>
+    <row r="158" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="C158" s="5"/>
+    </row>
+    <row r="159" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B159" s="5"/>
+      <c r="C159" s="5"/>
+    </row>
+    <row r="160" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="C160" s="5"/>
+    </row>
+    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B161" s="5"/>
+      <c r="C161" s="5"/>
+    </row>
+    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="C162" s="5"/>
+    </row>
+    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B163" s="5"/>
+      <c r="C163" s="5"/>
+    </row>
+    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B164" s="5"/>
+      <c r="C164" s="5"/>
+    </row>
+    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B165" s="5"/>
+      <c r="C165" s="5"/>
+    </row>
+    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B166" s="5"/>
+      <c r="C166" s="5"/>
+    </row>
+    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B167" s="5"/>
+      <c r="C167" s="5"/>
+    </row>
+    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="C168" s="5"/>
+    </row>
+    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B169" s="5"/>
+      <c r="C169" s="5"/>
+    </row>
+    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B170" s="5"/>
+      <c r="C170" s="5"/>
+    </row>
+    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B171" s="5"/>
+      <c r="C171" s="5"/>
+    </row>
+    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B172" s="5"/>
+      <c r="C172" s="5"/>
+    </row>
+    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B173" s="5"/>
+      <c r="C173" s="5"/>
+    </row>
+    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B174" s="5"/>
+      <c r="C174" s="5"/>
+    </row>
+    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B175" s="5"/>
+      <c r="C175" s="5"/>
+    </row>
+    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B176" s="5"/>
+      <c r="C176" s="5"/>
+    </row>
+    <row r="177" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B177" s="5"/>
+      <c r="C177" s="5"/>
+    </row>
+    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B178" s="5"/>
+      <c r="C178" s="5"/>
+    </row>
+    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B179" s="5"/>
+      <c r="C179" s="5"/>
+    </row>
+    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B180" s="5"/>
+      <c r="C180" s="5"/>
+    </row>
+    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B181" s="5"/>
+      <c r="C181" s="5"/>
+    </row>
+    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B182" s="5"/>
+      <c r="C182" s="5"/>
+    </row>
+    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B183" s="5"/>
+      <c r="C183" s="5"/>
+    </row>
+    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="5"/>
+      <c r="C184" s="5"/>
+    </row>
+    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="5"/>
+      <c r="C185" s="5"/>
+    </row>
+    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="5"/>
+      <c r="C186" s="5"/>
+    </row>
+    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="5"/>
+      <c r="C187" s="5"/>
+    </row>
+    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="5"/>
+      <c r="C188" s="5"/>
+    </row>
+    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="5"/>
+      <c r="C189" s="5"/>
+    </row>
+    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="5"/>
+      <c r="C190" s="5"/>
+    </row>
+    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="5"/>
+      <c r="C191" s="5"/>
+    </row>
+    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="5"/>
+      <c r="C192" s="5"/>
+    </row>
+    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="5"/>
+      <c r="C193" s="5"/>
+    </row>
+    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="5"/>
+      <c r="C194" s="5"/>
+    </row>
+    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="5"/>
+      <c r="C195" s="5"/>
+    </row>
+    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="5"/>
+      <c r="C196" s="5"/>
+    </row>
+    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="5"/>
+      <c r="C197" s="5"/>
+    </row>
+    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="5"/>
+      <c r="C198" s="5"/>
+    </row>
+    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="5"/>
+      <c r="C199" s="5"/>
+    </row>
+    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="5"/>
+      <c r="C200" s="5"/>
+    </row>
+    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="5"/>
+      <c r="C201" s="5"/>
+    </row>
+    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="5"/>
+      <c r="C202" s="5"/>
+    </row>
+    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="5"/>
+      <c r="C203" s="5"/>
+    </row>
+    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="5"/>
+      <c r="C204" s="5"/>
+    </row>
+    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="5"/>
+      <c r="C205" s="5"/>
+    </row>
+    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="5"/>
+      <c r="C206" s="5"/>
+    </row>
+    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="5"/>
+      <c r="C207" s="5"/>
+    </row>
+    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="5"/>
+      <c r="C208" s="5"/>
+    </row>
+    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="5"/>
+      <c r="C209" s="5"/>
+    </row>
+    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="5"/>
+      <c r="C210" s="5"/>
+    </row>
+    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="5"/>
+      <c r="C211" s="5"/>
+    </row>
+    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="5"/>
+      <c r="C212" s="5"/>
+    </row>
+    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="5"/>
+      <c r="C213" s="5"/>
+    </row>
+    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="5"/>
+      <c r="C214" s="5"/>
+    </row>
+    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="5"/>
+      <c r="C215" s="5"/>
+    </row>
+    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="5"/>
+      <c r="C216" s="5"/>
+    </row>
+    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="5"/>
+      <c r="C217" s="5"/>
+    </row>
+    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="5"/>
+      <c r="C218" s="5"/>
+    </row>
+    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+    </row>
+    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="5"/>
+      <c r="C220" s="5"/>
+    </row>
+    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+    </row>
+    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+    </row>
+    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+    </row>
+    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="5"/>
+      <c r="C224" s="5"/>
+    </row>
+    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="5"/>
+      <c r="C225" s="5"/>
+    </row>
+    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="5"/>
+      <c r="C226" s="5"/>
+    </row>
+    <row r="227" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+    </row>
+    <row r="228" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+    </row>
+    <row r="229" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="5"/>
+      <c r="C229" s="5"/>
+    </row>
+    <row r="230" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="5"/>
+      <c r="C230" s="5"/>
+    </row>
+    <row r="231" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="5"/>
+      <c r="C231" s="5"/>
+    </row>
+    <row r="232" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+    </row>
+    <row r="233" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="5"/>
+      <c r="C233" s="5"/>
+    </row>
+    <row r="234" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="5"/>
+      <c r="C234" s="5"/>
+    </row>
+    <row r="235" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="5"/>
+      <c r="C235" s="5"/>
+    </row>
+    <row r="236" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="5"/>
+      <c r="C236" s="5"/>
+    </row>
+    <row r="237" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="5"/>
+      <c r="C237" s="5"/>
+    </row>
+    <row r="238" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="5"/>
+      <c r="C238" s="5"/>
+    </row>
+    <row r="239" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="5"/>
+      <c r="C239" s="5"/>
+    </row>
+    <row r="240" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="5"/>
+      <c r="C240" s="5"/>
+    </row>
+    <row r="241" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="5"/>
+      <c r="C241" s="5"/>
+    </row>
+    <row r="242" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="5"/>
+      <c r="C242" s="5"/>
+    </row>
+    <row r="243" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="5"/>
+      <c r="C243" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>